<commit_message>
update to game data
</commit_message>
<xml_diff>
--- a/game_data_final/Barceloneta - Jug.xlsx
+++ b/game_data_final/Barceloneta - Jug.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="66">
   <si>
     <t>Number of Passes</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>Kickout Position</t>
+  </si>
+  <si>
+    <t>End 3-3</t>
   </si>
   <si>
     <t>5m</t>
@@ -212,9 +215,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m-d"/>
-  </numFmts>
   <fonts count="4">
     <font>
       <sz val="10.0"/>
@@ -244,14 +244,11 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -361,14 +358,14 @@
       <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="2">
-        <v>43527.0</v>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA1" s="3" t="s">
         <v>25</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="2">
@@ -376,7 +373,7 @@
         <v>8.0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D2" s="1">
         <v>1.0</v>
@@ -391,7 +388,7 @@
         <v>1.0</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I2" s="1">
         <v>0.0</v>
@@ -400,10 +397,10 @@
         <v>0.0</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N2" s="1">
         <v>4.0</v>
@@ -412,13 +409,13 @@
         <v>1.0</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Q2" s="1">
         <v>0.0</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="S2" s="1">
         <v>0.0</v>
@@ -426,10 +423,10 @@
       <c r="T2" s="1">
         <v>1.0</v>
       </c>
-      <c r="U2" s="4">
+      <c r="U2" s="3">
         <v>0.20069444444444445</v>
       </c>
-      <c r="V2" s="4">
+      <c r="V2" s="3">
         <v>0.18541666666666667</v>
       </c>
       <c r="W2" s="1">
@@ -444,8 +441,8 @@
       <c r="Z2" s="1">
         <v>0.0</v>
       </c>
-      <c r="AA2" s="5" t="s">
-        <v>32</v>
+      <c r="AA2" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="3">
@@ -453,7 +450,7 @@
         <v>9.0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D3" s="1">
         <v>1.0</v>
@@ -468,7 +465,7 @@
         <v>0.0</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I3" s="1">
         <v>0.0</v>
@@ -477,10 +474,10 @@
         <v>0.0</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N3" s="1">
         <v>5.0</v>
@@ -489,13 +486,13 @@
         <v>1.0</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Q3" s="1">
         <v>0.0</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="S3" s="1">
         <v>0.0</v>
@@ -503,10 +500,10 @@
       <c r="T3" s="1">
         <v>1.0</v>
       </c>
-      <c r="U3" s="4">
+      <c r="U3" s="3">
         <v>0.17708333333333334</v>
       </c>
-      <c r="V3" s="4">
+      <c r="V3" s="3">
         <v>0.16527777777777777</v>
       </c>
       <c r="W3" s="1">
@@ -521,8 +518,8 @@
       <c r="Z3" s="1">
         <v>0.0</v>
       </c>
-      <c r="AA3" s="5" t="s">
-        <v>38</v>
+      <c r="AA3" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="4">
@@ -530,7 +527,7 @@
         <v>9.0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D4" s="1">
         <v>3.0</v>
@@ -545,7 +542,7 @@
         <v>0.0</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I4" s="1">
         <v>0.0</v>
@@ -554,10 +551,10 @@
         <v>0.0</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="N4" s="1">
         <v>4.0</v>
@@ -566,13 +563,13 @@
         <v>1.0</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Q4" s="1">
         <v>1.0</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="S4" s="1">
         <v>0.0</v>
@@ -580,10 +577,10 @@
       <c r="T4" s="1">
         <v>1.0</v>
       </c>
-      <c r="U4" s="4">
+      <c r="U4" s="3">
         <v>0.03263888888888889</v>
       </c>
-      <c r="V4" s="4">
+      <c r="V4" s="3">
         <v>0.017361111111111112</v>
       </c>
       <c r="W4" s="1">
@@ -598,8 +595,8 @@
       <c r="Z4" s="1">
         <v>0.0</v>
       </c>
-      <c r="AA4" s="5" t="s">
-        <v>43</v>
+      <c r="AA4" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="5">
@@ -607,7 +604,7 @@
         <v>5.0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D5" s="1">
         <v>1.0</v>
@@ -622,7 +619,7 @@
         <v>1.0</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I5" s="1">
         <v>1.0</v>
@@ -631,10 +628,10 @@
         <v>0.0</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N5" s="1">
         <v>4.0</v>
@@ -646,7 +643,7 @@
         <v>0.0</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="S5" s="1">
         <v>0.0</v>
@@ -654,10 +651,10 @@
       <c r="T5" s="1">
         <v>2.0</v>
       </c>
-      <c r="U5" s="4">
+      <c r="U5" s="3">
         <v>0.27291666666666664</v>
       </c>
-      <c r="V5" s="4">
+      <c r="V5" s="3">
         <v>0.25972222222222224</v>
       </c>
       <c r="W5" s="1">
@@ -672,8 +669,8 @@
       <c r="Z5" s="1">
         <v>0.0</v>
       </c>
-      <c r="AA5" s="5" t="s">
-        <v>45</v>
+      <c r="AA5" s="4" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="6">
@@ -681,7 +678,7 @@
         <v>9.0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D6" s="1">
         <v>1.0</v>
@@ -696,7 +693,7 @@
         <v>1.0</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I6" s="1">
         <v>1.0</v>
@@ -705,10 +702,10 @@
         <v>0.0</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N6" s="1">
         <v>4.0</v>
@@ -717,13 +714,13 @@
         <v>1.0</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="Q6" s="1">
         <v>0.0</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="S6" s="1">
         <v>0.0</v>
@@ -731,10 +728,10 @@
       <c r="T6" s="1">
         <v>2.0</v>
       </c>
-      <c r="U6" s="4">
+      <c r="U6" s="3">
         <v>0.12638888888888888</v>
       </c>
-      <c r="V6" s="4">
+      <c r="V6" s="3">
         <v>0.1111111111111111</v>
       </c>
       <c r="W6" s="1">
@@ -749,8 +746,8 @@
       <c r="Z6" s="1">
         <v>0.0</v>
       </c>
-      <c r="AA6" s="5" t="s">
-        <v>49</v>
+      <c r="AA6" s="4" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="7">
@@ -758,7 +755,7 @@
         <v>8.0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D7" s="1">
         <v>5.0</v>
@@ -773,7 +770,7 @@
         <v>1.0</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I7" s="1">
         <v>1.0</v>
@@ -782,10 +779,10 @@
         <v>0.0</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N7" s="1">
         <v>4.0</v>
@@ -794,13 +791,13 @@
         <v>1.0</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="Q7" s="1">
         <v>1.0</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="S7" s="1">
         <v>0.0</v>
@@ -808,10 +805,10 @@
       <c r="T7" s="1">
         <v>2.0</v>
       </c>
-      <c r="U7" s="4">
+      <c r="U7" s="3">
         <v>0.09236111111111112</v>
       </c>
-      <c r="V7" s="4">
+      <c r="V7" s="3">
         <v>0.07916666666666666</v>
       </c>
       <c r="W7" s="1">
@@ -826,8 +823,8 @@
       <c r="Z7" s="1">
         <v>0.0</v>
       </c>
-      <c r="AA7" s="5" t="s">
-        <v>52</v>
+      <c r="AA7" s="4" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="8">
@@ -835,7 +832,7 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D8" s="1">
         <v>1.0</v>
@@ -850,7 +847,7 @@
         <v>0.0</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I8" s="1">
         <v>0.0</v>
@@ -859,10 +856,10 @@
         <v>0.0</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N8" s="1">
         <v>4.0</v>
@@ -871,13 +868,13 @@
         <v>1.0</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="Q8" s="1">
         <v>1.0</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="S8" s="1">
         <v>0.0</v>
@@ -885,10 +882,10 @@
       <c r="T8" s="1">
         <v>2.0</v>
       </c>
-      <c r="U8" s="4">
+      <c r="U8" s="3">
         <v>0.02361111111111111</v>
       </c>
-      <c r="V8" s="4">
+      <c r="V8" s="3">
         <v>0.008333333333333333</v>
       </c>
       <c r="W8" s="1">
@@ -903,8 +900,8 @@
       <c r="Z8" s="1">
         <v>0.0</v>
       </c>
-      <c r="AA8" s="5" t="s">
-        <v>55</v>
+      <c r="AA8" s="4" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="9">
@@ -912,7 +909,7 @@
         <v>6.0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D9" s="1">
         <v>1.0</v>
@@ -927,7 +924,7 @@
         <v>0.0</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I9" s="1">
         <v>0.0</v>
@@ -936,10 +933,10 @@
         <v>0.0</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="N9" s="1">
         <v>6.0</v>
@@ -948,13 +945,13 @@
         <v>1.0</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="Q9" s="1">
         <v>0.0</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="S9" s="1">
         <v>0.0</v>
@@ -962,10 +959,10 @@
       <c r="T9" s="1">
         <v>4.0</v>
       </c>
-      <c r="U9" s="4">
+      <c r="U9" s="3">
         <v>0.25625</v>
       </c>
-      <c r="V9" s="4">
+      <c r="V9" s="3">
         <v>0.23819444444444443</v>
       </c>
       <c r="W9" s="1">
@@ -980,8 +977,8 @@
       <c r="Z9" s="1">
         <v>0.0</v>
       </c>
-      <c r="AA9" s="5" t="s">
-        <v>58</v>
+      <c r="AA9" s="4" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="10">
@@ -989,7 +986,7 @@
         <v>11.0</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D10" s="1">
         <v>6.0</v>
@@ -1004,7 +1001,7 @@
         <v>0.0</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I10" s="1">
         <v>0.0</v>
@@ -1013,10 +1010,10 @@
         <v>0.0</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N10" s="1">
         <v>5.0</v>
@@ -1025,13 +1022,13 @@
         <v>1.0</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="Q10" s="1">
         <v>0.0</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="S10" s="1">
         <v>0.0</v>
@@ -1039,10 +1036,10 @@
       <c r="T10" s="1">
         <v>4.0</v>
       </c>
-      <c r="U10" s="4">
+      <c r="U10" s="3">
         <v>0.21805555555555556</v>
       </c>
-      <c r="V10" s="4">
+      <c r="V10" s="3">
         <v>0.2013888888888889</v>
       </c>
       <c r="W10" s="1">
@@ -1057,8 +1054,8 @@
       <c r="Z10" s="1">
         <v>0.0</v>
       </c>
-      <c r="AA10" s="5" t="s">
-        <v>61</v>
+      <c r="AA10" s="4" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="11">
@@ -1066,13 +1063,13 @@
         <v>7.0</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F11" s="1">
         <v>0.0</v>
@@ -1081,7 +1078,7 @@
         <v>0.0</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I11" s="1">
         <v>0.0</v>
@@ -1090,25 +1087,25 @@
         <v>0.0</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="Q11" s="1">
         <v>1.0</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="S11" s="1">
         <v>1.0</v>
@@ -1116,10 +1113,10 @@
       <c r="T11" s="1">
         <v>4.0</v>
       </c>
-      <c r="U11" s="4">
+      <c r="U11" s="3">
         <v>0.16319444444444445</v>
       </c>
-      <c r="V11" s="4">
+      <c r="V11" s="3">
         <v>0.15</v>
       </c>
       <c r="W11" s="1">
@@ -1134,8 +1131,8 @@
       <c r="Z11" s="1">
         <v>0.0</v>
       </c>
-      <c r="AA11" s="5" t="s">
-        <v>64</v>
+      <c r="AA11" s="4" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>